<commit_message>
Update to schema and fix Makefile
</commit_message>
<xml_diff>
--- a/project/excel/sepio_linkml.xlsx
+++ b/project/excel/sepio_linkml.xlsx
@@ -489,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,60 +585,65 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -650,137 +655,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>focus</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>dataItems</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>interpretation</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sourceDataSet</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>componentResult</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>studyGroup</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>isAbout</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>contributions</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>dateAuthored</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>specifiedBy</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>methodTypes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>derivedFrom</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>reportedIn</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>informationQuality</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>recordMetadata</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>identifiers</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>alternativeLabels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -797,6 +671,142 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>focus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dataItems</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>interpretation</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sourceDataSet</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>componentResult</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>studyGroup</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>isAbout</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>contributions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dateAuthored</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>specifiedBy</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>supportingMethods</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>reportedIn</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>informationQuality</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>recordMetadata</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>identifiers</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>alternativeLabels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>subtype</t>
         </is>
       </c>
@@ -852,60 +862,65 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -1241,7 +1256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1272,60 +1287,65 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -1424,7 +1444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1465,60 +1485,65 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -1535,7 +1560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1596,60 +1621,65 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -1666,7 +1696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1727,60 +1757,65 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
@@ -1797,7 +1832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1848,60 +1883,65 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>methodTypes</t>
+          <t>supportingMethods</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>supportingMethodTypes</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>derivedFrom</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>reportedIn</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>informationQuality</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>recordMetadata</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>identifiers</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>alternativeLabels</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>

</xml_diff>